<commit_message>
Dont Allow Dash while Upload.. Remove dash from rings in existing data..
</commit_message>
<xml_diff>
--- a/src/scripts/export.xlsx
+++ b/src/scripts/export.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Vendor</t>
   </si>
@@ -59,10 +59,13 @@
     <t>Style Code</t>
   </si>
   <si>
-    <t>CM-SDC3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dia Bead - ROUND shape Polki double sided - 8mm </t>
+    <t>RG006719</t>
+  </si>
+  <si>
+    <t>14YR785.7</t>
+  </si>
+  <si>
+    <t>14K Rings- Dia Yellow XOXO ring</t>
   </si>
 </sst>
 </file>
@@ -513,40 +516,44 @@
     </row>
     <row r="2" spans="1:14" customHeight="1" ht="82.5">
       <c r="A2">
-        <v>161</v>
-      </c>
-      <c r="B2"/>
+        <v>199</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2"/>
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
       <c r="G2">
-        <v>1.3</v>
+        <v>1.685</v>
       </c>
       <c r="H2">
-        <v>0.25</v>
+        <v>0.118</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
+        <v>1.661</v>
+      </c>
+      <c r="K2">
         <v>0</v>
       </c>
-      <c r="K2">
-        <v>14</v>
-      </c>
       <c r="L2">
-        <v>47</v>
+        <v>348</v>
       </c>
       <c r="M2">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <v>10</v>
+        <v>586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>